<commit_message>
general utility for camp
</commit_message>
<xml_diff>
--- a/QSP/resources/tdforWriteMsg.xlsx
+++ b/QSP/resources/tdforWriteMsg.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="47">
   <si>
     <t>TestCase</t>
   </si>
@@ -151,6 +151,14 @@
   </si>
   <si>
     <t>Product iphoneNeetu817 Successfully Added</t>
+  </si>
+  <si>
+    <t>Product iphoneNeetu208 Successfully Added
+✖︎</t>
+  </si>
+  <si>
+    <t>Product iphoneNeetu904 Successfully Added
+✖︎</t>
   </si>
 </sst>
 </file>
@@ -637,7 +645,7 @@
         <v>41</v>
       </c>
       <c r="E2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>